<commit_message>
Updated with changes from Amazon Skill Certification Testing
</commit_message>
<xml_diff>
--- a/Skill_Details.xlsx
+++ b/Skill_Details.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Skill Information" sheetId="2" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="17">
   <si>
     <t>Keywords:</t>
   </si>
@@ -28,18 +28,9 @@
     <t>Example Phrases:</t>
   </si>
   <si>
-    <t>What's the dial code for Greece</t>
-  </si>
-  <si>
     <t>Full Skill Description</t>
   </si>
   <si>
-    <t xml:space="preserve">You can ask Alex to tell you the dial code needed for any country in the world.  </t>
-  </si>
-  <si>
-    <t>Shor Skill Description</t>
-  </si>
-  <si>
     <t>Category</t>
   </si>
   <si>
@@ -58,10 +49,25 @@
     <t>Sub Category</t>
   </si>
   <si>
-    <t>Alexa, what's the dial code for China</t>
-  </si>
-  <si>
-    <t>What's the dial code for France</t>
+    <t>Alexa, ask country dial codes what's the dial code for China.</t>
+  </si>
+  <si>
+    <t>What's the phone code for France?</t>
+  </si>
+  <si>
+    <t>What's the code for Greece?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You can ask Alexa to tell you the dial code needed for any country in the world.  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">This skill enables Alexa to tell you the dial code needed to call a given country.  </t>
+  </si>
+  <si>
+    <t>Short Skill Description</t>
+  </si>
+  <si>
+    <t>Lookup, Country, Code, Prefix, Phone</t>
   </si>
 </sst>
 </file>
@@ -97,8 +103,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -108,6 +117,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -285,7 +297,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -320,7 +332,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -559,84 +571,87 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:C10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="20.140625" customWidth="1"/>
-    <col min="3" max="3" width="73.7109375" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="20.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="73.7109375" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C2" t="s">
+    </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B7" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
+    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C8" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C3" t="s">
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C9" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
-        <v>2</v>
-      </c>
-      <c r="C7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C8" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C9" t="s">
-        <v>14</v>
-      </c>
-    </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
+      <c r="B10" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C10" t="s">
-        <v>1</v>
+      <c r="C10" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -644,7 +659,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>

</xml_diff>